<commit_message>
Code refactoring: - Moves the http execution to test_suite_ctx. - Test result is now computed from TestSuiteCtx
</commit_message>
<xml_diff>
--- a/data/ngage-tests.xlsx
+++ b/data/ngage-tests.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -86,6 +86,11 @@
   </si>
   <si>
     <t xml:space="preserve">globals.email = "ravindranath.m@comviva.co.in"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAT.test("Response status shalt be 400", () =&gt; {
+  return SAT.response.status == 400;
+});</t>
   </si>
   <si>
     <t xml:space="preserve">Sign up with missing email field</t>
@@ -402,8 +407,8 @@
   </sheetPr>
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.0078125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -412,7 +417,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="25.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="21.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="24.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="24.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.18"/>
@@ -420,7 +425,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="45.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="13" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="48.87"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="14" style="1" width="21"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -464,7 +470,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -494,6 +500,9 @@
       </c>
       <c r="L2" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="58.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -501,7 +510,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
@@ -519,7 +528,7 @@
         <v>18</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J3" s="1" t="n">
         <v>400</v>
@@ -530,10 +539,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>15</v>
@@ -548,7 +557,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>400</v>
@@ -559,16 +568,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>17</v>
@@ -577,7 +586,7 @@
         <v>18</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>201</v>
@@ -588,10 +597,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="72.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -599,16 +608,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>17</v>
@@ -617,7 +626,7 @@
         <v>18</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J7" s="1" t="n">
         <v>201</v>
@@ -628,16 +637,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>17</v>
@@ -646,7 +655,7 @@
         <v>18</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J8" s="1" t="n">
         <v>409</v>
@@ -654,7 +663,7 @@
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>

</xml_diff>

<commit_message>
Donno what this nonsense is...  I don't understand this merge conflicts stuff.
</commit_message>
<xml_diff>
--- a/data/ngage-tests.xlsx
+++ b/data/ngage-tests.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravindranath.m\projects\satyanaash\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravindranath.m\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FE1479-3220-486A-9B68-82B8AD859489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F124F562-A6F5-4F7E-8AE5-FE4DFB833503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>id</t>
   </si>
@@ -105,12 +105,6 @@
     <t>It should fail with 400 status</t>
   </si>
   <si>
-    <t>{
-  "email": "user@example.com",
-  "company": "kabra-ka-idabra"
-}</t>
-  </si>
-  <si>
     <t>Sign up with missing email field</t>
   </si>
   <si>
@@ -172,7 +166,22 @@
     <t>post-test script</t>
   </si>
   <si>
-    <t>variables.username = "Ravindranath"</t>
+    <t>globals.email = "Ravindranath";
+globals.company = "my_com";</t>
+  </si>
+  <si>
+    <t>{
+  "email": "{{email}}",
+  "company": "{{company}}"
+}</t>
+  </si>
+  <si>
+    <t>content-type: application/json, user-agent: curl/7.64.1</t>
+  </si>
+  <si>
+    <t>SAT.test("Response should match with 400", ()=&gt; {
+  return SAT.response.status == 400;
+})</t>
   </si>
 </sst>
 </file>
@@ -600,7 +609,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21" defaultRowHeight="14.65" x14ac:dyDescent="1.5"/>
@@ -612,9 +621,9 @@
     <col min="5" max="5" width="24.52734375" style="4" customWidth="1"/>
     <col min="6" max="6" width="8.3515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.64453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.17578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.17578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.64453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.9375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="34.46875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="8.64453125" style="2" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="10.76171875" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="21" style="2"/>
   </cols>
@@ -653,14 +662,14 @@
       <c r="K1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="58.9" thickTop="1" x14ac:dyDescent="1.5">
+    </row>
+    <row r="2" spans="1:13" ht="102.75" thickTop="1" x14ac:dyDescent="1.5">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -682,14 +691,20 @@
       <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="H2" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="I2" s="4" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="J2" s="2">
         <v>400</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>39</v>
+      <c r="L2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="58.5" x14ac:dyDescent="1.5">
@@ -697,7 +712,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>19</v>
@@ -715,7 +730,7 @@
         <v>4</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" s="2">
         <v>400</v>
@@ -726,10 +741,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>15</v>
@@ -744,7 +759,7 @@
         <v>4</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" s="2">
         <v>400</v>
@@ -784,10 +799,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="73.150000000000006" x14ac:dyDescent="1.5">
@@ -795,16 +810,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>16</v>
@@ -813,7 +828,7 @@
         <v>4</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J7" s="2">
         <v>201</v>
@@ -824,16 +839,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>16</v>
@@ -842,7 +857,7 @@
         <v>4</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J8" s="2">
         <v>409</v>
@@ -850,7 +865,7 @@
     </row>
     <row r="9" spans="1:13" ht="24" x14ac:dyDescent="1.5">
       <c r="B9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>

</xml_diff>